<commit_message>
Added a Continent column on each dfataframe Replaced void cells with zeroes. Merged Luxembourg rows and updated Belgium.
</commit_message>
<xml_diff>
--- a/datasets/1a - Total production.xlsx
+++ b/datasets/1a - Total production.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Drive\Data analysis projects\Coffee_production_consumption\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A65C5BF2-D6CF-4B5E-AB00-6938ACCED8FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0688258B-D902-48D8-9430-DCD7018BF909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="95">
   <si>
     <t>Total production by all exporting countries</t>
   </si>
@@ -286,9 +286,6 @@
     <t>Total</t>
   </si>
   <si>
-    <t>Crop year</t>
-  </si>
-  <si>
     <t>2015/16</t>
   </si>
   <si>
@@ -301,9 +298,6 @@
     <t>2018/19</t>
   </si>
   <si>
-    <t>Bolivia (Plurinational State of)</t>
-  </si>
-  <si>
     <t>Congo</t>
   </si>
   <si>
@@ -332,6 +326,12 @@
   </si>
   <si>
     <t>Group</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Bolivia</t>
   </si>
 </sst>
 </file>
@@ -2235,13 +2235,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AF98"/>
+  <dimension ref="A1:AG98"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="P5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B59" sqref="B4:B59"/>
+      <selection pane="bottomRight" activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -2252,29 +2252,29 @@
     <col min="33" max="16384" width="8.85546875" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="15"/>
       <c r="C1" s="16"/>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="16"/>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A3" s="6"/>
     </row>
-    <row r="4" spans="1:32" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>3</v>
@@ -2352,27 +2352,30 @@
         <v>27</v>
       </c>
       <c r="AB4" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC4" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="AC4" s="3" t="s">
+      <c r="AD4" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="AD4" s="3" t="s">
+      <c r="AE4" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="AE4" s="3" t="s">
-        <v>83</v>
-      </c>
       <c r="AF4" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
+        <v>88</v>
+      </c>
+      <c r="AG4" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C5" s="8">
         <v>50.344999999999999</v>
@@ -2464,13 +2467,17 @@
       <c r="AF5" s="9">
         <v>51.841900000000003</v>
       </c>
-    </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG5" s="9">
+        <f>SUM(C5:AF5)</f>
+        <v>1365.7826</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C6" s="8">
         <v>122.777</v>
@@ -2562,13 +2569,17 @@
       <c r="AF6" s="9">
         <v>81.2654</v>
       </c>
-    </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG6" s="9">
+        <f t="shared" ref="AG6:AG61" si="0">SUM(C6:AF6)</f>
+        <v>3449.5030999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>29</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C7" s="8">
         <v>27285.6286</v>
@@ -2660,13 +2671,17 @@
       <c r="AF7" s="9">
         <v>58210.712699999996</v>
       </c>
-    </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG7" s="9">
+        <f t="shared" si="0"/>
+        <v>1251382.3185000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>30</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C8" s="8">
         <v>487.39299999999997</v>
@@ -2758,13 +2773,17 @@
       <c r="AF8" s="9">
         <v>272.46879999999999</v>
       </c>
-    </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG8" s="9">
+        <f t="shared" si="0"/>
+        <v>10396.362999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>31</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C9" s="8">
         <v>1503.8150000000001</v>
@@ -2856,13 +2875,17 @@
       <c r="AF9" s="9">
         <v>558.93520000000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG9" s="9">
+        <f t="shared" si="0"/>
+        <v>31672.561400000006</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>32</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C10" s="8">
         <v>7441.3829999999998</v>
@@ -2954,13 +2977,17 @@
       <c r="AF10" s="9">
         <v>11432.942499999999</v>
       </c>
-    </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG10" s="9">
+        <f t="shared" si="0"/>
+        <v>256749.71320000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>33</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C11" s="8">
         <v>982.447</v>
@@ -3052,13 +3079,17 @@
       <c r="AF11" s="9">
         <v>383.3125</v>
       </c>
-    </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG11" s="9">
+        <f t="shared" si="0"/>
+        <v>17426.543600000005</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>34</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C12" s="8">
         <v>104.628</v>
@@ -3150,13 +3181,17 @@
       <c r="AF12" s="9">
         <v>16.043099999999999</v>
       </c>
-    </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG12" s="9">
+        <f t="shared" si="0"/>
+        <v>1370.8337999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>35</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C13" s="8">
         <v>962.84100000000001</v>
@@ -3248,13 +3283,17 @@
       <c r="AF13" s="9">
         <v>751.721</v>
       </c>
-    </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG13" s="9">
+        <f t="shared" si="0"/>
+        <v>30051.428900000006</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>36</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C14" s="8">
         <v>130.62700000000001</v>
@@ -3346,13 +3385,17 @@
       <c r="AF14" s="9">
         <v>20.003799999999998</v>
       </c>
-    </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG14" s="9">
+        <f t="shared" si="0"/>
+        <v>1035.8646999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>37</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C15" s="8">
         <v>936.63199999999995</v>
@@ -3444,13 +3487,17 @@
       <c r="AF15" s="9">
         <v>3836.3816999999999</v>
       </c>
-    </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG15" s="9">
+        <f t="shared" si="0"/>
+        <v>88627.052100000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C16" s="8">
         <v>534.875</v>
@@ -3542,13 +3589,17 @@
       <c r="AF16" s="9">
         <v>347.98399999999998</v>
       </c>
-    </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG16" s="9">
+        <f t="shared" si="0"/>
+        <v>9457.4567000000025</v>
+      </c>
+    </row>
+    <row r="17" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>39</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C17" s="8">
         <v>0</v>
@@ -3640,13 +3691,17 @@
       <c r="AF17" s="9">
         <v>103.0527</v>
       </c>
-    </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG17" s="9">
+        <f t="shared" si="0"/>
+        <v>1143.4122000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>40</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C18" s="8">
         <v>251.90100000000001</v>
@@ -3738,13 +3793,17 @@
       <c r="AF18" s="9">
         <v>9.0784000000000002</v>
       </c>
-    </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG18" s="9">
+        <f t="shared" si="0"/>
+        <v>2203.851900000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C19" s="8">
         <v>2.9239999999999999</v>
@@ -3836,13 +3895,17 @@
       <c r="AF19" s="9">
         <v>3.0005999999999999</v>
       </c>
-    </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG19" s="9">
+        <f t="shared" si="0"/>
+        <v>114.58370000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>41</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C20" s="8">
         <v>414.21199999999999</v>
@@ -3934,13 +3997,17 @@
       <c r="AF20" s="9">
         <v>130.18289999999999</v>
       </c>
-    </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG20" s="9">
+        <f t="shared" si="0"/>
+        <v>5987.277100000003</v>
+      </c>
+    </row>
+    <row r="21" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>42</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C21" s="8">
         <v>880.06200000000001</v>
@@ -4032,13 +4099,17 @@
       <c r="AF21" s="9">
         <v>401.63479999999998</v>
       </c>
-    </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG21" s="9">
+        <f t="shared" si="0"/>
+        <v>15157.507900000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>43</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C22" s="8">
         <v>392.88</v>
@@ -4130,13 +4201,17 @@
       <c r="AF22" s="9">
         <v>346.64949999999999</v>
       </c>
-    </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG22" s="9">
+        <f t="shared" si="0"/>
+        <v>11646.973000000004</v>
+      </c>
+    </row>
+    <row r="23" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>44</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C23" s="8">
         <v>973.63199999999995</v>
@@ -4228,13 +4303,17 @@
       <c r="AF23" s="9">
         <v>306.53440000000001</v>
       </c>
-    </row>
-    <row r="24" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG23" s="9">
+        <f t="shared" si="0"/>
+        <v>14843.433400000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>45</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C24" s="8">
         <v>931.779</v>
@@ -4326,13 +4405,17 @@
       <c r="AF24" s="9">
         <v>926.39250000000004</v>
       </c>
-    </row>
-    <row r="25" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG24" s="9">
+        <f t="shared" si="0"/>
+        <v>24579.262600000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>46</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C25" s="8">
         <v>22.686</v>
@@ -4424,13 +4507,17 @@
       <c r="AF25" s="9">
         <v>14.5428</v>
       </c>
-    </row>
-    <row r="26" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG25" s="9">
+        <f t="shared" si="0"/>
+        <v>1281.0475000000004</v>
+      </c>
+    </row>
+    <row r="26" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>47</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C26" s="8">
         <v>1682.4839999999999</v>
@@ -4522,13 +4609,17 @@
       <c r="AF26" s="9">
         <v>268.209</v>
       </c>
-    </row>
-    <row r="27" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG26" s="9">
+        <f t="shared" si="0"/>
+        <v>22644.342099999994</v>
+      </c>
+    </row>
+    <row r="27" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>48</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C27" s="8">
         <v>175.274</v>
@@ -4620,13 +4711,17 @@
       <c r="AF27" s="9">
         <v>55.138300000000001</v>
       </c>
-    </row>
-    <row r="28" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG27" s="9">
+        <f t="shared" si="0"/>
+        <v>3065.7106000000003</v>
+      </c>
+    </row>
+    <row r="28" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>49</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C28" s="8">
         <v>14396</v>
@@ -4718,13 +4813,17 @@
       <c r="AF28" s="9">
         <v>14100.118200000001</v>
       </c>
-    </row>
-    <row r="29" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG28" s="9">
+        <f t="shared" si="0"/>
+        <v>359979.56460000004</v>
+      </c>
+    </row>
+    <row r="29" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>50</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C29" s="8">
         <v>2561.8850000000002</v>
@@ -4816,13 +4915,17 @@
       <c r="AF29" s="9">
         <v>1471.7632000000001</v>
       </c>
-    </row>
-    <row r="30" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG29" s="9">
+        <f t="shared" si="0"/>
+        <v>59941.651699999995</v>
+      </c>
+    </row>
+    <row r="30" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>51</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C30" s="8">
         <v>2940.3629999999998</v>
@@ -4914,13 +5017,17 @@
       <c r="AF30" s="9">
         <v>1929.1972000000001</v>
       </c>
-    </row>
-    <row r="31" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG30" s="9">
+        <f t="shared" si="0"/>
+        <v>79357.411300000022</v>
+      </c>
+    </row>
+    <row r="31" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C31" s="8">
         <v>1580.296</v>
@@ -5012,13 +5119,17 @@
       <c r="AF31" s="9">
         <v>390.60140000000001</v>
       </c>
-    </row>
-    <row r="32" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG31" s="9">
+        <f t="shared" si="0"/>
+        <v>17516.602299999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>52</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C32" s="8">
         <v>2464.864</v>
@@ -5110,13 +5221,17 @@
       <c r="AF32" s="9">
         <v>660.69159999999999</v>
       </c>
-    </row>
-    <row r="33" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG32" s="9">
+        <f t="shared" si="0"/>
+        <v>47013.837299999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>53</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C33" s="8">
         <v>3.536</v>
@@ -5208,13 +5323,17 @@
       <c r="AF33" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG33" s="9">
+        <f t="shared" si="0"/>
+        <v>16.835000000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>54</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C34" s="8">
         <v>2909.451</v>
@@ -5306,13 +5425,17 @@
       <c r="AF34" s="9">
         <v>7343.4328999999998</v>
       </c>
-    </row>
-    <row r="35" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG34" s="9">
+        <f t="shared" si="0"/>
+        <v>144494.32599999994</v>
+      </c>
+    </row>
+    <row r="35" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>55</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C35" s="8">
         <v>3.4079999999999999</v>
@@ -5404,13 +5527,17 @@
       <c r="AF35" s="9">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="36" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG35" s="9">
+        <f t="shared" si="0"/>
+        <v>45.187100000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
         <v>56</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C36" s="8">
         <v>37.854999999999997</v>
@@ -5502,13 +5629,17 @@
       <c r="AF36" s="9">
         <v>14.4733</v>
       </c>
-    </row>
-    <row r="37" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG36" s="9">
+        <f t="shared" si="0"/>
+        <v>1063.6336000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
         <v>57</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C37" s="8">
         <v>3270.529</v>
@@ -5600,13 +5731,17 @@
       <c r="AF37" s="9">
         <v>3605.7644</v>
       </c>
-    </row>
-    <row r="38" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG37" s="9">
+        <f t="shared" si="0"/>
+        <v>117006.83459999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
         <v>58</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C38" s="8">
         <v>44.46</v>
@@ -5698,13 +5833,17 @@
       <c r="AF38" s="9">
         <v>178.37790000000001</v>
       </c>
-    </row>
-    <row r="39" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG38" s="9">
+        <f t="shared" si="0"/>
+        <v>8041.0969999999998</v>
+      </c>
+    </row>
+    <row r="39" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
         <v>59</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C39" s="8">
         <v>0</v>
@@ -5796,13 +5935,17 @@
       <c r="AF39" s="9">
         <v>9.5059000000000005</v>
       </c>
-    </row>
-    <row r="40" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG39" s="9">
+        <f t="shared" si="0"/>
+        <v>179.72599999999997</v>
+      </c>
+    </row>
+    <row r="40" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>60</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C40" s="8">
         <v>1567.9580000000001</v>
@@ -5894,13 +6037,17 @@
       <c r="AF40" s="9">
         <v>5931.22</v>
       </c>
-    </row>
-    <row r="41" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG40" s="9">
+        <f t="shared" si="0"/>
+        <v>111212.80880000001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>61</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C41" s="8">
         <v>2828.6869999999999</v>
@@ -5992,13 +6139,17 @@
       <c r="AF41" s="9">
         <v>4987.6264000000001</v>
       </c>
-    </row>
-    <row r="42" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG41" s="9">
+        <f t="shared" si="0"/>
+        <v>137036.30739999999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
         <v>62</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C42" s="8">
         <v>22.574000000000002</v>
@@ -6090,13 +6241,17 @@
       <c r="AF42" s="9">
         <v>22.879300000000001</v>
       </c>
-    </row>
-    <row r="43" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG42" s="9">
+        <f t="shared" si="0"/>
+        <v>899.13779999999997</v>
+      </c>
+    </row>
+    <row r="43" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
         <v>63</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C43" s="8">
         <v>1485.135</v>
@@ -6188,13 +6343,17 @@
       <c r="AF43" s="9">
         <v>843.7079</v>
       </c>
-    </row>
-    <row r="44" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG43" s="9">
+        <f t="shared" si="0"/>
+        <v>29471.561400000002</v>
+      </c>
+    </row>
+    <row r="44" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C44" s="8">
         <v>0</v>
@@ -6286,13 +6445,17 @@
       <c r="AF44" s="9">
         <v>621.84460000000001</v>
       </c>
-    </row>
-    <row r="45" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG44" s="9">
+        <f t="shared" si="0"/>
+        <v>9470.0369999999984</v>
+      </c>
+    </row>
+    <row r="45" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
         <v>64</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C45" s="8">
         <v>3</v>
@@ -6384,13 +6547,17 @@
       <c r="AF45" s="9">
         <v>5.85</v>
       </c>
-    </row>
-    <row r="46" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG45" s="9">
+        <f t="shared" si="0"/>
+        <v>249.49809999999997</v>
+      </c>
+    </row>
+    <row r="46" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
         <v>65</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C46" s="8">
         <v>4674.2449999999999</v>
@@ -6482,13 +6649,17 @@
       <c r="AF46" s="9">
         <v>3984.6010999999999</v>
       </c>
-    </row>
-    <row r="47" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG46" s="9">
+        <f t="shared" si="0"/>
+        <v>130892.84779999997</v>
+      </c>
+    </row>
+    <row r="47" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
         <v>66</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C47" s="8">
         <v>0</v>
@@ -6580,13 +6751,17 @@
       <c r="AF47" s="9">
         <v>0.69430000000000003</v>
       </c>
-    </row>
-    <row r="48" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG47" s="9">
+        <f t="shared" si="0"/>
+        <v>25.377499999999998</v>
+      </c>
+    </row>
+    <row r="48" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
         <v>67</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C48" s="8">
         <v>461.07799999999997</v>
@@ -6678,13 +6853,17 @@
       <c r="AF48" s="9">
         <v>2882.3199</v>
       </c>
-    </row>
-    <row r="49" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG48" s="9">
+        <f t="shared" si="0"/>
+        <v>45824.506300000001</v>
+      </c>
+    </row>
+    <row r="49" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
         <v>68</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C49" s="8">
         <v>29.19</v>
@@ -6776,13 +6955,17 @@
       <c r="AF49" s="9">
         <v>42.469499999999996</v>
       </c>
-    </row>
-    <row r="50" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG49" s="9">
+        <f t="shared" si="0"/>
+        <v>1366.0042999999994</v>
+      </c>
+    </row>
+    <row r="50" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
         <v>69</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C50" s="8">
         <v>214.98699999999999</v>
@@ -6874,13 +7057,17 @@
       <c r="AF50" s="9">
         <v>114.4053</v>
       </c>
-    </row>
-    <row r="51" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG50" s="9">
+        <f t="shared" si="0"/>
+        <v>4684.5447000000013</v>
+      </c>
+    </row>
+    <row r="51" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
         <v>70</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C51" s="8">
         <v>42.783000000000001</v>
@@ -6972,13 +7159,17 @@
       <c r="AF51" s="9">
         <v>39.987099999999998</v>
       </c>
-    </row>
-    <row r="52" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG51" s="9">
+        <f t="shared" si="0"/>
+        <v>1452.3503999999998</v>
+      </c>
+    </row>
+    <row r="52" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
         <v>71</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C52" s="8">
         <v>95.87</v>
@@ -7070,13 +7261,17 @@
       <c r="AF52" s="9">
         <v>36.218699999999998</v>
       </c>
-    </row>
-    <row r="53" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG52" s="9">
+        <f t="shared" si="0"/>
+        <v>1228.4842999999998</v>
+      </c>
+    </row>
+    <row r="53" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
         <v>72</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C53" s="8">
         <v>757.01700000000005</v>
@@ -7168,13 +7363,17 @@
       <c r="AF53" s="9">
         <v>516.57830000000001</v>
       </c>
-    </row>
-    <row r="54" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG53" s="9">
+        <f t="shared" si="0"/>
+        <v>27900.515300000006</v>
+      </c>
+    </row>
+    <row r="54" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
         <v>73</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C54" s="11">
         <v>161.30799999999999</v>
@@ -7266,13 +7465,17 @@
       <c r="AF54" s="9">
         <v>40.616999999999997</v>
       </c>
-    </row>
-    <row r="55" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG54" s="9">
+        <f t="shared" si="0"/>
+        <v>4689.8741</v>
+      </c>
+    </row>
+    <row r="55" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
         <v>74</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C55" s="11">
         <v>14.581</v>
@@ -7364,13 +7567,17 @@
       <c r="AF55" s="9">
         <v>11.691000000000001</v>
       </c>
-    </row>
-    <row r="56" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG55" s="9">
+        <f t="shared" si="0"/>
+        <v>430.74589999999995</v>
+      </c>
+    </row>
+    <row r="56" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
         <v>75</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C56" s="11">
         <v>1955.009</v>
@@ -7462,13 +7669,17 @@
       <c r="AF56" s="9">
         <v>5509.1540000000005</v>
       </c>
-    </row>
-    <row r="57" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG56" s="9">
+        <f t="shared" si="0"/>
+        <v>98655.523000000001</v>
+      </c>
+    </row>
+    <row r="57" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
         <v>76</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C57" s="11">
         <v>1122.4770000000001</v>
@@ -7560,13 +7771,17 @@
       <c r="AF57" s="9">
         <v>650.1046</v>
       </c>
-    </row>
-    <row r="58" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG57" s="9">
+        <f t="shared" si="0"/>
+        <v>33213.356399999997</v>
+      </c>
+    </row>
+    <row r="58" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C58" s="11">
         <v>1310.288</v>
@@ -7658,13 +7873,17 @@
       <c r="AF58" s="9">
         <v>30487.164400000001</v>
       </c>
-    </row>
-    <row r="59" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG58" s="9">
+        <f t="shared" si="0"/>
+        <v>480054.97269999998</v>
+      </c>
+    </row>
+    <row r="59" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
         <v>77</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C59" s="11">
         <v>0</v>
@@ -7756,99 +7975,104 @@
       <c r="AF59" s="9">
         <v>91.427800000000005</v>
       </c>
-    </row>
-    <row r="60" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG59" s="9">
+        <f t="shared" si="0"/>
+        <v>3182.6585</v>
+      </c>
+    </row>
+    <row r="60" spans="1:33" x14ac:dyDescent="0.2">
       <c r="B60" s="10"/>
       <c r="C60" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D60" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E60" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F60" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G60" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H60" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I60" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J60" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="K60" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="L60" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="M60" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="N60" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="O60" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="P60" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="Q60" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="R60" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="S60" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="T60" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="U60" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="V60" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="W60" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="X60" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="Y60" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="Z60" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="AA60" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="AB60" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="AC60" s="9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="AD60" s="9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="AE60" s="9"/>
       <c r="AF60" s="9" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="61" spans="1:32" s="16" customFormat="1" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+      <c r="AG60" s="9"/>
+    </row>
+    <row r="61" spans="1:33" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A61" s="12" t="s">
         <v>78</v>
       </c>
@@ -7943,8 +8167,12 @@
       <c r="AF61" s="14">
         <v>165053.01570000002</v>
       </c>
-    </row>
-    <row r="62" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG61" s="9">
+        <f t="shared" si="0"/>
+        <v>3762250.6418000003</v>
+      </c>
+    </row>
+    <row r="62" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
         <v>2</v>
       </c>
@@ -7973,8 +8201,9 @@
       <c r="Y62" s="5"/>
       <c r="Z62" s="5"/>
       <c r="AA62" s="5"/>
-    </row>
-    <row r="63" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG62" s="9"/>
+    </row>
+    <row r="63" spans="1:33" x14ac:dyDescent="0.2">
       <c r="C63" s="5"/>
       <c r="D63" s="5"/>
       <c r="E63" s="5"/>
@@ -8001,7 +8230,7 @@
       <c r="Z63" s="5"/>
       <c r="AA63" s="5"/>
     </row>
-    <row r="64" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:33" x14ac:dyDescent="0.2">
       <c r="N64" s="9"/>
     </row>
     <row r="65" spans="14:14" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Added barcharts and cloropleth maps
</commit_message>
<xml_diff>
--- a/datasets/1a - Total production.xlsx
+++ b/datasets/1a - Total production.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Drive\Data analysis projects\Coffee_production_consumption\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D7B5C56-6234-4FC0-B701-EC2688FC318E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5454B209-C544-405A-937B-5FE37FFFBEC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Production" sheetId="1" r:id="rId1"/>
@@ -307,9 +307,6 @@
     <t>Lao People's Democratic Republic</t>
   </si>
   <si>
-    <t>Viet Nam</t>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
@@ -335,6 +332,9 @@
   </si>
   <si>
     <t>Totals</t>
+  </si>
+  <si>
+    <t>Vietnam</t>
   </si>
 </sst>
 </file>
@@ -2241,10 +2241,10 @@
   <dimension ref="A1:AG98"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="Q5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="Q29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AG4" sqref="AG4"/>
+      <selection pane="bottomRight" activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -2274,10 +2274,10 @@
     </row>
     <row r="4" spans="1:33" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>3</v>
@@ -2367,10 +2367,10 @@
         <v>82</v>
       </c>
       <c r="AF4" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AG4" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.2">
@@ -2378,7 +2378,7 @@
         <v>28</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C5" s="8">
         <v>50.344999999999999</v>
@@ -2477,10 +2477,10 @@
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C6" s="8">
         <v>122.777</v>
@@ -2582,7 +2582,7 @@
         <v>29</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C7" s="8">
         <v>27285.6286</v>
@@ -2684,7 +2684,7 @@
         <v>30</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C8" s="8">
         <v>487.39299999999997</v>
@@ -2786,7 +2786,7 @@
         <v>31</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C9" s="8">
         <v>1503.8150000000001</v>
@@ -2888,7 +2888,7 @@
         <v>32</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C10" s="8">
         <v>7441.3829999999998</v>
@@ -2990,7 +2990,7 @@
         <v>33</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C11" s="8">
         <v>982.447</v>
@@ -3092,7 +3092,7 @@
         <v>34</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C12" s="8">
         <v>104.628</v>
@@ -3194,7 +3194,7 @@
         <v>35</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C13" s="8">
         <v>962.84100000000001</v>
@@ -3296,7 +3296,7 @@
         <v>36</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C14" s="8">
         <v>130.62700000000001</v>
@@ -3398,7 +3398,7 @@
         <v>37</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C15" s="8">
         <v>936.63199999999995</v>
@@ -3500,7 +3500,7 @@
         <v>38</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C16" s="8">
         <v>534.875</v>
@@ -3602,7 +3602,7 @@
         <v>39</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C17" s="8">
         <v>0</v>
@@ -3704,7 +3704,7 @@
         <v>40</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C18" s="8">
         <v>251.90100000000001</v>
@@ -3806,7 +3806,7 @@
         <v>83</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C19" s="8">
         <v>2.9239999999999999</v>
@@ -3908,7 +3908,7 @@
         <v>41</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C20" s="8">
         <v>414.21199999999999</v>
@@ -4010,7 +4010,7 @@
         <v>42</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C21" s="8">
         <v>880.06200000000001</v>
@@ -4112,7 +4112,7 @@
         <v>43</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C22" s="8">
         <v>392.88</v>
@@ -4214,7 +4214,7 @@
         <v>44</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C23" s="8">
         <v>973.63199999999995</v>
@@ -4316,7 +4316,7 @@
         <v>45</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C24" s="8">
         <v>931.779</v>
@@ -4418,7 +4418,7 @@
         <v>46</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C25" s="8">
         <v>22.686</v>
@@ -4520,7 +4520,7 @@
         <v>47</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C26" s="8">
         <v>1682.4839999999999</v>
@@ -4622,7 +4622,7 @@
         <v>48</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C27" s="8">
         <v>175.274</v>
@@ -4724,7 +4724,7 @@
         <v>49</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C28" s="8">
         <v>14396</v>
@@ -4826,7 +4826,7 @@
         <v>50</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C29" s="8">
         <v>2561.8850000000002</v>
@@ -4928,7 +4928,7 @@
         <v>51</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C30" s="8">
         <v>2940.3629999999998</v>
@@ -5030,7 +5030,7 @@
         <v>84</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C31" s="8">
         <v>1580.296</v>
@@ -5132,7 +5132,7 @@
         <v>52</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C32" s="8">
         <v>2464.864</v>
@@ -5234,7 +5234,7 @@
         <v>53</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C33" s="8">
         <v>3.536</v>
@@ -5336,7 +5336,7 @@
         <v>54</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C34" s="8">
         <v>2909.451</v>
@@ -5438,7 +5438,7 @@
         <v>55</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C35" s="8">
         <v>3.4079999999999999</v>
@@ -5540,7 +5540,7 @@
         <v>56</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C36" s="8">
         <v>37.854999999999997</v>
@@ -5642,7 +5642,7 @@
         <v>57</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C37" s="8">
         <v>3270.529</v>
@@ -5744,7 +5744,7 @@
         <v>58</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C38" s="8">
         <v>44.46</v>
@@ -5846,7 +5846,7 @@
         <v>59</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C39" s="8">
         <v>0</v>
@@ -5948,7 +5948,7 @@
         <v>60</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C40" s="8">
         <v>1567.9580000000001</v>
@@ -6050,7 +6050,7 @@
         <v>61</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C41" s="8">
         <v>2828.6869999999999</v>
@@ -6152,7 +6152,7 @@
         <v>62</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C42" s="8">
         <v>22.574000000000002</v>
@@ -6254,7 +6254,7 @@
         <v>63</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C43" s="8">
         <v>1485.135</v>
@@ -6356,7 +6356,7 @@
         <v>85</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C44" s="8">
         <v>0</v>
@@ -6458,7 +6458,7 @@
         <v>64</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C45" s="8">
         <v>3</v>
@@ -6560,7 +6560,7 @@
         <v>65</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C46" s="8">
         <v>4674.2449999999999</v>
@@ -6662,7 +6662,7 @@
         <v>66</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C47" s="8">
         <v>0</v>
@@ -6764,7 +6764,7 @@
         <v>67</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C48" s="8">
         <v>461.07799999999997</v>
@@ -6866,7 +6866,7 @@
         <v>68</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C49" s="8">
         <v>29.19</v>
@@ -6968,7 +6968,7 @@
         <v>69</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C50" s="8">
         <v>214.98699999999999</v>
@@ -7070,7 +7070,7 @@
         <v>70</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C51" s="8">
         <v>42.783000000000001</v>
@@ -7172,7 +7172,7 @@
         <v>71</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C52" s="8">
         <v>95.87</v>
@@ -7274,7 +7274,7 @@
         <v>72</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C53" s="8">
         <v>757.01700000000005</v>
@@ -7376,7 +7376,7 @@
         <v>73</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C54" s="11">
         <v>161.30799999999999</v>
@@ -7478,7 +7478,7 @@
         <v>74</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C55" s="11">
         <v>14.581</v>
@@ -7580,7 +7580,7 @@
         <v>75</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C56" s="11">
         <v>1955.009</v>
@@ -7682,7 +7682,7 @@
         <v>76</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C57" s="11">
         <v>1122.4770000000001</v>
@@ -7781,10 +7781,10 @@
     </row>
     <row r="58" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C58" s="11">
         <v>1310.288</v>
@@ -7886,7 +7886,7 @@
         <v>77</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C59" s="11">
         <v>0</v>
@@ -7986,92 +7986,92 @@
     <row r="60" spans="1:33" x14ac:dyDescent="0.2">
       <c r="B60" s="10"/>
       <c r="C60" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D60" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E60" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F60" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G60" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H60" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I60" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J60" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K60" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L60" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="M60" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="N60" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="O60" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="P60" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="Q60" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="R60" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="S60" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="T60" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="U60" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="V60" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="W60" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="X60" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="Y60" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="Z60" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AA60" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AB60" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AC60" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AD60" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AE60" s="9"/>
       <c r="AF60" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AG60" s="9"/>
     </row>

</xml_diff>

<commit_message>
Updated files and streamlit dashboard main.py
</commit_message>
<xml_diff>
--- a/datasets/1a - Total production.xlsx
+++ b/datasets/1a - Total production.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Drive\Data analysis projects\Coffee_production_consumption\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF6B6BDA-7ABC-4E70-AFAD-5C57F628DCBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC9CB648-094A-433E-9D11-0D0B4F0FCF4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -217,9 +217,6 @@
     <t>Democratic Republic of Congo</t>
   </si>
   <si>
-    <t>Lao People's Democratic Republic</t>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
@@ -335,6 +332,9 @@
   </si>
   <si>
     <t>2019</t>
+  </si>
+  <si>
+    <t>Laos</t>
   </si>
 </sst>
 </file>
@@ -2244,7 +2244,7 @@
       <pane xSplit="1" ySplit="4" topLeftCell="B29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="C4" sqref="C4:AF4"/>
+      <selection pane="bottomRight" activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -2274,103 +2274,103 @@
     </row>
     <row r="4" spans="1:33" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="J4" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="M4" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="N4" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="O4" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="O4" s="3" t="s">
+      <c r="P4" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="P4" s="3" t="s">
+      <c r="Q4" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="Q4" s="3" t="s">
+      <c r="R4" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="R4" s="3" t="s">
+      <c r="S4" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="S4" s="3" t="s">
+      <c r="T4" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="T4" s="3" t="s">
+      <c r="U4" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="U4" s="3" t="s">
+      <c r="V4" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="V4" s="3" t="s">
+      <c r="W4" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="W4" s="3" t="s">
+      <c r="X4" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="X4" s="3" t="s">
+      <c r="Y4" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="Y4" s="3" t="s">
+      <c r="Z4" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="Z4" s="3" t="s">
+      <c r="AA4" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="AA4" s="3" t="s">
+      <c r="AB4" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="AB4" s="3" t="s">
+      <c r="AC4" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="AC4" s="3" t="s">
+      <c r="AD4" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="AD4" s="3" t="s">
+      <c r="AE4" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="AE4" s="3" t="s">
+      <c r="AF4" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="AF4" s="3" t="s">
-        <v>95</v>
-      </c>
       <c r="AG4" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.2">
@@ -2378,7 +2378,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C5" s="8">
         <v>50.344999999999999</v>
@@ -2477,10 +2477,10 @@
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C6" s="8">
         <v>122.777</v>
@@ -2582,7 +2582,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C7" s="8">
         <v>27285.6286</v>
@@ -2684,7 +2684,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C8" s="8">
         <v>487.39299999999997</v>
@@ -2786,7 +2786,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C9" s="8">
         <v>1503.8150000000001</v>
@@ -2888,7 +2888,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C10" s="8">
         <v>7441.3829999999998</v>
@@ -2990,7 +2990,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C11" s="8">
         <v>982.447</v>
@@ -3092,7 +3092,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C12" s="8">
         <v>104.628</v>
@@ -3194,7 +3194,7 @@
         <v>10</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C13" s="8">
         <v>962.84100000000001</v>
@@ -3296,7 +3296,7 @@
         <v>11</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C14" s="8">
         <v>130.62700000000001</v>
@@ -3398,7 +3398,7 @@
         <v>12</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C15" s="8">
         <v>936.63199999999995</v>
@@ -3500,7 +3500,7 @@
         <v>13</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C16" s="8">
         <v>534.875</v>
@@ -3602,7 +3602,7 @@
         <v>14</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C17" s="8">
         <v>0</v>
@@ -3704,7 +3704,7 @@
         <v>15</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C18" s="8">
         <v>251.90100000000001</v>
@@ -3806,7 +3806,7 @@
         <v>54</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C19" s="8">
         <v>2.9239999999999999</v>
@@ -3908,7 +3908,7 @@
         <v>16</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C20" s="8">
         <v>414.21199999999999</v>
@@ -4010,7 +4010,7 @@
         <v>17</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C21" s="8">
         <v>880.06200000000001</v>
@@ -4112,7 +4112,7 @@
         <v>18</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C22" s="8">
         <v>392.88</v>
@@ -4214,7 +4214,7 @@
         <v>19</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C23" s="8">
         <v>973.63199999999995</v>
@@ -4316,7 +4316,7 @@
         <v>20</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C24" s="8">
         <v>931.779</v>
@@ -4418,7 +4418,7 @@
         <v>21</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C25" s="8">
         <v>22.686</v>
@@ -4520,7 +4520,7 @@
         <v>22</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C26" s="8">
         <v>1682.4839999999999</v>
@@ -4622,7 +4622,7 @@
         <v>23</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C27" s="8">
         <v>175.274</v>
@@ -4724,7 +4724,7 @@
         <v>24</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C28" s="8">
         <v>14396</v>
@@ -4826,7 +4826,7 @@
         <v>25</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C29" s="8">
         <v>2561.8850000000002</v>
@@ -4928,7 +4928,7 @@
         <v>26</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C30" s="8">
         <v>2940.3629999999998</v>
@@ -5030,7 +5030,7 @@
         <v>55</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C31" s="8">
         <v>1580.296</v>
@@ -5132,7 +5132,7 @@
         <v>27</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C32" s="8">
         <v>2464.864</v>
@@ -5234,7 +5234,7 @@
         <v>28</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C33" s="8">
         <v>3.536</v>
@@ -5336,7 +5336,7 @@
         <v>29</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C34" s="8">
         <v>2909.451</v>
@@ -5438,7 +5438,7 @@
         <v>30</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C35" s="8">
         <v>3.4079999999999999</v>
@@ -5540,7 +5540,7 @@
         <v>31</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C36" s="8">
         <v>37.854999999999997</v>
@@ -5642,7 +5642,7 @@
         <v>32</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C37" s="8">
         <v>3270.529</v>
@@ -5744,7 +5744,7 @@
         <v>33</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C38" s="8">
         <v>44.46</v>
@@ -5846,7 +5846,7 @@
         <v>34</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C39" s="8">
         <v>0</v>
@@ -5948,7 +5948,7 @@
         <v>35</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C40" s="8">
         <v>1567.9580000000001</v>
@@ -6050,7 +6050,7 @@
         <v>36</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C41" s="8">
         <v>2828.6869999999999</v>
@@ -6152,7 +6152,7 @@
         <v>37</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C42" s="8">
         <v>22.574000000000002</v>
@@ -6254,7 +6254,7 @@
         <v>38</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C43" s="8">
         <v>1485.135</v>
@@ -6353,10 +6353,10 @@
     </row>
     <row r="44" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
-        <v>56</v>
+        <v>95</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C44" s="8">
         <v>0</v>
@@ -6458,7 +6458,7 @@
         <v>39</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C45" s="8">
         <v>3</v>
@@ -6560,7 +6560,7 @@
         <v>40</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C46" s="8">
         <v>4674.2449999999999</v>
@@ -6662,7 +6662,7 @@
         <v>41</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C47" s="8">
         <v>0</v>
@@ -6764,7 +6764,7 @@
         <v>42</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C48" s="8">
         <v>461.07799999999997</v>
@@ -6866,7 +6866,7 @@
         <v>43</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C49" s="8">
         <v>29.19</v>
@@ -6968,7 +6968,7 @@
         <v>44</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C50" s="8">
         <v>214.98699999999999</v>
@@ -7070,7 +7070,7 @@
         <v>45</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C51" s="8">
         <v>42.783000000000001</v>
@@ -7172,7 +7172,7 @@
         <v>46</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C52" s="8">
         <v>95.87</v>
@@ -7274,7 +7274,7 @@
         <v>47</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C53" s="8">
         <v>757.01700000000005</v>
@@ -7376,7 +7376,7 @@
         <v>48</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C54" s="11">
         <v>161.30799999999999</v>
@@ -7478,7 +7478,7 @@
         <v>49</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C55" s="11">
         <v>14.581</v>
@@ -7580,7 +7580,7 @@
         <v>50</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C56" s="11">
         <v>1955.009</v>
@@ -7682,7 +7682,7 @@
         <v>51</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C57" s="11">
         <v>1122.4770000000001</v>
@@ -7781,10 +7781,10 @@
     </row>
     <row r="58" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C58" s="11">
         <v>1310.288</v>
@@ -7886,7 +7886,7 @@
         <v>52</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C59" s="11">
         <v>0</v>
@@ -7986,92 +7986,92 @@
     <row r="60" spans="1:33" x14ac:dyDescent="0.2">
       <c r="B60" s="10"/>
       <c r="C60" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D60" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E60" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F60" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G60" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H60" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I60" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J60" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K60" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L60" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M60" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="N60" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="O60" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P60" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Q60" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="R60" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="S60" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="T60" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="U60" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="V60" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="W60" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="X60" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Y60" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Z60" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AA60" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AB60" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AC60" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AD60" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AE60" s="9"/>
       <c r="AF60" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AG60" s="9"/>
     </row>

</xml_diff>